<commit_message>
Update URLs in configuration and resources
</commit_message>
<xml_diff>
--- a/temp/pages/StructureDefinition-my-patient.xlsx
+++ b/temp/pages/StructureDefinition-my-patient.xlsx
@@ -27,7 +27,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://example.org//StructureDefinition/my-patient</t>
+    <t>http://example.org/StructureDefinition/my-patient</t>
   </si>
   <si>
     <t>Version</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-08T14:05:39+01:00</t>
+    <t>2024-03-08T14:42:37+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -447,7 +447,7 @@
     <t>favoriteColor</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://example.org//StructureDefinition/favorite-color}
+    <t xml:space="preserve">Extension {http://example.org/StructureDefinition/favorite-color}
 </t>
   </si>
   <si>
@@ -1928,7 +1928,7 @@
     <col min="8" max="8" width="14.7109375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="60.85546875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="59.89453125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
Update URLs in ImplementationGuide and StructureDefinition
</commit_message>
<xml_diff>
--- a/temp/pages/StructureDefinition-my-patient.xlsx
+++ b/temp/pages/StructureDefinition-my-patient.xlsx
@@ -27,7 +27,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://example.org/StructureDefinition/my-patient</t>
+    <t>http://example.org/fhir/ImplementationGuide/cs6440/StructureDefinition/my-patient</t>
   </si>
   <si>
     <t>Version</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-08T14:46:34+01:00</t>
+    <t>2024-03-08T15:26:18+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -447,7 +447,7 @@
     <t>favoriteColor</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://example.org/StructureDefinition/favorite-color}
+    <t xml:space="preserve">Extension {http://example.org/fhir/ImplementationGuide/cs6440/StructureDefinition/favorite-color}
 </t>
   </si>
   <si>
@@ -1928,7 +1928,7 @@
     <col min="8" max="8" width="14.7109375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="59.89453125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="91.54296875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>